<commit_message>
Added corrrected activity-diagrams and updated time-planning
</commit_message>
<xml_diff>
--- a/Documentation/Planung/Projektplanung.xlsx
+++ b/Documentation/Planung/Projektplanung.xlsx
@@ -637,7 +637,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gesamtübersicht - Zeitbedarfsüb'!$B$4:$D$4</c:f>
+              <c:f>'Gesamtübersicht - Zeitbedarfsüb'!$B$4,'Gesamtübersicht - Zeitbedarfsüb'!$C$4,'Gesamtübersicht - Zeitbedarfsüb'!$D$4</c:f>
               <c:numCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1278,7 +1278,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 2 - Meilenstein 2'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 2 - Meilenstein 2'!$F$5,'Meilenstein 2 - Meilenstein 2'!$F$6,'Meilenstein 2 - Meilenstein 2'!$F$7,'Meilenstein 2 - Meilenstein 2'!$F$8,'Meilenstein 2 - Meilenstein 2'!$F$9,'Meilenstein 2 - Meilenstein 2'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -1873,7 +1873,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 2 - Meilenstein 2'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 2 - Meilenstein 2'!$H$5,'Meilenstein 2 - Meilenstein 2'!$H$6,'Meilenstein 2 - Meilenstein 2'!$H$7,'Meilenstein 2 - Meilenstein 2'!$H$8,'Meilenstein 2 - Meilenstein 2'!$H$9,'Meilenstein 2 - Meilenstein 2'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -2468,7 +2468,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 3a - Meilenstein 3a'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 3a - Meilenstein 3a'!$D$5,'Meilenstein 3a - Meilenstein 3a'!$D$6,'Meilenstein 3a - Meilenstein 3a'!$D$7,'Meilenstein 3a - Meilenstein 3a'!$D$8,'Meilenstein 3a - Meilenstein 3a'!$D$9,'Meilenstein 3a - Meilenstein 3a'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -3063,7 +3063,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 3a - Meilenstein 3a'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 3a - Meilenstein 3a'!$F$5,'Meilenstein 3a - Meilenstein 3a'!$F$6,'Meilenstein 3a - Meilenstein 3a'!$F$7,'Meilenstein 3a - Meilenstein 3a'!$F$8,'Meilenstein 3a - Meilenstein 3a'!$F$9,'Meilenstein 3a - Meilenstein 3a'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -3658,7 +3658,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 3a - Meilenstein 3a'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 3a - Meilenstein 3a'!$H$5,'Meilenstein 3a - Meilenstein 3a'!$H$6,'Meilenstein 3a - Meilenstein 3a'!$H$7,'Meilenstein 3a - Meilenstein 3a'!$H$8,'Meilenstein 3a - Meilenstein 3a'!$H$9,'Meilenstein 3a - Meilenstein 3a'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -4253,7 +4253,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 3b - Meilenstein 3b'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 3b - Meilenstein 3b'!$D$5,'Meilenstein 3b - Meilenstein 3b'!$D$6,'Meilenstein 3b - Meilenstein 3b'!$D$7,'Meilenstein 3b - Meilenstein 3b'!$D$8,'Meilenstein 3b - Meilenstein 3b'!$D$9,'Meilenstein 3b - Meilenstein 3b'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -4848,7 +4848,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 3b - Meilenstein 3b'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 3b - Meilenstein 3b'!$F$5,'Meilenstein 3b - Meilenstein 3b'!$F$6,'Meilenstein 3b - Meilenstein 3b'!$F$7,'Meilenstein 3b - Meilenstein 3b'!$F$8,'Meilenstein 3b - Meilenstein 3b'!$F$9,'Meilenstein 3b - Meilenstein 3b'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -5443,7 +5443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 3b - Meilenstein 3b'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 3b - Meilenstein 3b'!$H$5,'Meilenstein 3b - Meilenstein 3b'!$H$6,'Meilenstein 3b - Meilenstein 3b'!$H$7,'Meilenstein 3b - Meilenstein 3b'!$H$8,'Meilenstein 3b - Meilenstein 3b'!$H$9,'Meilenstein 3b - Meilenstein 3b'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -6038,7 +6038,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 4 - Meilenstein 4'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 4 - Meilenstein 4'!$D$5,'Meilenstein 4 - Meilenstein 4'!$D$6,'Meilenstein 4 - Meilenstein 4'!$D$7,'Meilenstein 4 - Meilenstein 4'!$D$8,'Meilenstein 4 - Meilenstein 4'!$D$9,'Meilenstein 4 - Meilenstein 4'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -6633,7 +6633,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 4 - Meilenstein 4'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 4 - Meilenstein 4'!$F$5,'Meilenstein 4 - Meilenstein 4'!$F$6,'Meilenstein 4 - Meilenstein 4'!$F$7,'Meilenstein 4 - Meilenstein 4'!$F$8,'Meilenstein 4 - Meilenstein 4'!$F$9,'Meilenstein 4 - Meilenstein 4'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -7021,17 +7021,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gesamtübersicht - Zeitbedarfsüb'!$B$5:$D$5</c:f>
+              <c:f>'Gesamtübersicht - Zeitbedarfsüb'!$B$5,'Gesamtübersicht - Zeitbedarfsüb'!$C$5,'Gesamtübersicht - Zeitbedarfsüb'!$D$5</c:f>
               <c:numCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.670000</c:v>
+                  <c:v>12.170000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.700000</c:v>
+                  <c:v>11.950000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7662,7 +7662,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 4 - Meilenstein 4'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 4 - Meilenstein 4'!$H$5,'Meilenstein 4 - Meilenstein 4'!$H$6,'Meilenstein 4 - Meilenstein 4'!$H$7,'Meilenstein 4 - Meilenstein 4'!$H$8,'Meilenstein 4 - Meilenstein 4'!$H$9,'Meilenstein 4 - Meilenstein 4'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -8257,7 +8257,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 5 - Meilenstein 5'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 5 - Meilenstein 5'!$D$5,'Meilenstein 5 - Meilenstein 5'!$D$6,'Meilenstein 5 - Meilenstein 5'!$D$7,'Meilenstein 5 - Meilenstein 5'!$D$8,'Meilenstein 5 - Meilenstein 5'!$D$9,'Meilenstein 5 - Meilenstein 5'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -8852,7 +8852,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 5 - Meilenstein 5'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 5 - Meilenstein 5'!$F$5,'Meilenstein 5 - Meilenstein 5'!$F$6,'Meilenstein 5 - Meilenstein 5'!$F$7,'Meilenstein 5 - Meilenstein 5'!$F$8,'Meilenstein 5 - Meilenstein 5'!$F$9,'Meilenstein 5 - Meilenstein 5'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -9447,7 +9447,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 5 - Meilenstein 5'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 5 - Meilenstein 5'!$H$5,'Meilenstein 5 - Meilenstein 5'!$H$6,'Meilenstein 5 - Meilenstein 5'!$H$7,'Meilenstein 5 - Meilenstein 5'!$H$8,'Meilenstein 5 - Meilenstein 5'!$H$9,'Meilenstein 5 - Meilenstein 5'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -10042,7 +10042,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 6 - Meilenstein 6'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 6 - Meilenstein 6'!$D$5,'Meilenstein 6 - Meilenstein 6'!$D$6,'Meilenstein 6 - Meilenstein 6'!$D$7,'Meilenstein 6 - Meilenstein 6'!$D$8,'Meilenstein 6 - Meilenstein 6'!$D$9,'Meilenstein 6 - Meilenstein 6'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -10637,7 +10637,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 6 - Meilenstein 6'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 6 - Meilenstein 6'!$F$5,'Meilenstein 6 - Meilenstein 6'!$F$6,'Meilenstein 6 - Meilenstein 6'!$F$7,'Meilenstein 6 - Meilenstein 6'!$F$8,'Meilenstein 6 - Meilenstein 6'!$F$9,'Meilenstein 6 - Meilenstein 6'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -11232,7 +11232,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 6 - Meilenstein 6'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 6 - Meilenstein 6'!$H$5,'Meilenstein 6 - Meilenstein 6'!$H$6,'Meilenstein 6 - Meilenstein 6'!$H$7,'Meilenstein 6 - Meilenstein 6'!$H$8,'Meilenstein 6 - Meilenstein 6'!$H$9,'Meilenstein 6 - Meilenstein 6'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -11827,7 +11827,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 1a - Meilenstein 1a'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 1a - Meilenstein 1a'!$D$5,'Meilenstein 1a - Meilenstein 1a'!$D$6,'Meilenstein 1a - Meilenstein 1a'!$D$7,'Meilenstein 1a - Meilenstein 1a'!$D$8,'Meilenstein 1a - Meilenstein 1a'!$D$9,'Meilenstein 1a - Meilenstein 1a'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="1">
@@ -12425,14 +12425,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 1a - Meilenstein 1a'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 1a - Meilenstein 1a'!$F$5,'Meilenstein 1a - Meilenstein 1a'!$F$6,'Meilenstein 1a - Meilenstein 1a'!$F$7,'Meilenstein 1a - Meilenstein 1a'!$F$8,'Meilenstein 1a - Meilenstein 1a'!$F$9,'Meilenstein 1a - Meilenstein 1a'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="1">
                   <c:v>5.250000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.420000</c:v>
+                  <c:v>6.920000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13026,14 +13026,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 1a - Meilenstein 1a'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 1a - Meilenstein 1a'!$H$5,'Meilenstein 1a - Meilenstein 1a'!$H$6,'Meilenstein 1a - Meilenstein 1a'!$H$7,'Meilenstein 1a - Meilenstein 1a'!$H$8,'Meilenstein 1a - Meilenstein 1a'!$H$9,'Meilenstein 1a - Meilenstein 1a'!$H$10</c:f>
               <c:numCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.700000</c:v>
+                  <c:v>5.700000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.250000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13627,7 +13630,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 1b - Meilenstein 1b'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 1b - Meilenstein 1b'!$D$5,'Meilenstein 1b - Meilenstein 1b'!$D$6,'Meilenstein 1b - Meilenstein 1b'!$D$7,'Meilenstein 1b - Meilenstein 1b'!$D$8,'Meilenstein 1b - Meilenstein 1b'!$D$9,'Meilenstein 1b - Meilenstein 1b'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -14222,7 +14225,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 1b - Meilenstein 1b'!$F$5:$F$10</c:f>
+              <c:f>'Meilenstein 1b - Meilenstein 1b'!$F$5,'Meilenstein 1b - Meilenstein 1b'!$F$6,'Meilenstein 1b - Meilenstein 1b'!$F$7,'Meilenstein 1b - Meilenstein 1b'!$F$8,'Meilenstein 1b - Meilenstein 1b'!$F$9,'Meilenstein 1b - Meilenstein 1b'!$F$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -14817,7 +14820,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 1b - Meilenstein 1b'!$H$5:$H$10</c:f>
+              <c:f>'Meilenstein 1b - Meilenstein 1b'!$H$5,'Meilenstein 1b - Meilenstein 1b'!$H$6,'Meilenstein 1b - Meilenstein 1b'!$H$7,'Meilenstein 1b - Meilenstein 1b'!$H$8,'Meilenstein 1b - Meilenstein 1b'!$H$9,'Meilenstein 1b - Meilenstein 1b'!$H$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -15412,7 +15415,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Meilenstein 2 - Meilenstein 2'!$D$5:$D$10</c:f>
+              <c:f>'Meilenstein 2 - Meilenstein 2'!$D$5,'Meilenstein 2 - Meilenstein 2'!$D$6,'Meilenstein 2 - Meilenstein 2'!$D$7,'Meilenstein 2 - Meilenstein 2'!$D$8,'Meilenstein 2 - Meilenstein 2'!$D$9,'Meilenstein 2 - Meilenstein 2'!$D$10</c:f>
               <c:numCache>
                 <c:ptCount val="0"/>
               </c:numCache>
@@ -17566,15 +17569,15 @@
       </c>
       <c r="C5" s="6">
         <f>SUM('Meilenstein 1a - Meilenstein 1a'!F12,'Meilenstein 1b - Meilenstein 1b'!F12,'Meilenstein 2 - Meilenstein 2'!F12,'Meilenstein 3a - Meilenstein 3a'!F12,'Meilenstein 3b - Meilenstein 3b'!F12,'Meilenstein 4 - Meilenstein 4'!F12,'Meilenstein 5 - Meilenstein 5'!F12,'Meilenstein 6 - Meilenstein 6'!F12)</f>
-        <v>6.67</v>
+        <v>12.17</v>
       </c>
       <c r="D5" s="6">
         <f>SUM('Meilenstein 1a - Meilenstein 1a'!H12,'Meilenstein 1b - Meilenstein 1b'!H12,'Meilenstein 2 - Meilenstein 2'!H12,'Meilenstein 3a - Meilenstein 3a'!H12,'Meilenstein 3b - Meilenstein 3b'!H12,'Meilenstein 4 - Meilenstein 4'!H12,'Meilenstein 5 - Meilenstein 5'!H12,'Meilenstein 6 - Meilenstein 6'!H12)</f>
-        <v>6.7</v>
+        <v>11.95</v>
       </c>
       <c r="E5" s="6">
         <f>SUM(B5:D5)</f>
-        <v>14.37</v>
+        <v>25.12</v>
       </c>
     </row>
   </sheetData>
@@ -17697,7 +17700,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="6">
-        <v>3.7</v>
+        <v>5.7</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="6">
@@ -17706,7 +17709,7 @@
       </c>
       <c r="K5" s="6">
         <f>SUM(D5,F5,H5)</f>
-        <v>3.7</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
@@ -17753,12 +17756,14 @@
         <v>5</v>
       </c>
       <c r="F7" s="6">
-        <v>1.42</v>
+        <v>6.92</v>
       </c>
       <c r="G7" s="6">
         <v>2</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6">
+        <v>3.25</v>
+      </c>
       <c r="I7" s="9"/>
       <c r="J7" s="6">
         <f>SUM(C7,E7,G7)</f>
@@ -17766,7 +17771,7 @@
       </c>
       <c r="K7" s="6">
         <f>SUM(D7,F7,H7)</f>
-        <v>1.42</v>
+        <v>10.17</v>
       </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
@@ -17877,7 +17882,7 @@
       </c>
       <c r="F12" s="10">
         <f>SUM(F5:F10)</f>
-        <v>6.67</v>
+        <v>12.17</v>
       </c>
       <c r="G12" s="10">
         <f>SUM(G5:G10)</f>
@@ -17885,7 +17890,7 @@
       </c>
       <c r="H12" s="10">
         <f>SUM(H5:H10)</f>
-        <v>6.7</v>
+        <v>11.95</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="10">
@@ -17894,16 +17899,16 @@
       </c>
       <c r="K12" s="10">
         <f>SUM(K5:K10)</f>
-        <v>14.37</v>
+        <v>25.12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -18214,10 +18219,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -18528,10 +18533,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -18842,10 +18847,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -19156,10 +19161,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -19470,10 +19475,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -19784,10 +19789,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -20098,10 +20103,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>